<commit_message>
Refactor and bug fix
</commit_message>
<xml_diff>
--- a/data/index_report.xlsx
+++ b/data/index_report.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI MO DE NOW TJX UNP INTU PGR WFC SYK COP LMT MU CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX BKNG TXN JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C TMO CME CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
+          <t>LLY V SPGI MDT NEE C CME APH MO BAC COF INTU LOW CVX ISRG BA BLK META CRM QCOM DHR NOW KKR BRK-B COST PG GILD AVGO ABBV ORCL CMCSA MCD PEP BKNG GEV BSX AMAT SYK DIS VZ CSCO LIN GOOGL ADP LRCX ANET JNJ T AMZN PLTR DE MU LMT VRTX AMGN TXN HD PM ETN KO IBM SCHW WMT HON ADI PGR GS NVDA MSFT WFC UBER PANW JPM GOOG AAPL MMC NFLX UNH RTX ABT MA UNP MS TJX ADBE AXP XOM TMO ICE CB COP CRWD MRK PFE TSLA CAT AMD GE TMUS ACN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -478,13 +478,13 @@
           <t>2025-06-02</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI MO DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX BKNG TXN JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C TMO CME CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C CME BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH MO COF ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -494,11 +494,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX BKNG TXN JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C TMO CME CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+          <t>KLAC</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C CME BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -508,11 +516,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX BKNG TXN JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+          <t>BX</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CME</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -522,11 +538,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW AMT TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX BKNG TXN JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+          <t>AMT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>BX</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -536,11 +560,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX BKNG TXN JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+          <t>BX</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>AMT</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -548,13 +580,13 @@
           <t>2025-06-07</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX BKNG TXN JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -562,13 +594,13 @@
           <t>2025-06-08</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX BKNG TXN JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -578,11 +610,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS PFE XOM MCD GE SBUX CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+          <t>SBUX</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ICE</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -590,13 +630,13 @@
           <t>2025-06-10</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS PFE XOM MCD GE SBUX CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -604,13 +644,13 @@
           <t>2025-06-11</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS PFE XOM MCD GE SBUX CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -620,11 +660,19 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS BMY PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+          <t>BMY</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BX</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -634,11 +682,19 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+          <t>ICE</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>BMY</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -646,13 +702,13 @@
           <t>2025-06-14</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -662,11 +718,19 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE BMY XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+          <t>BMY</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -676,11 +740,19 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>BMY</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -688,13 +760,13 @@
           <t>2025-06-17</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -702,13 +774,13 @@
           <t>2025-06-18</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -716,13 +788,13 @@
           <t>2025-06-19</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -730,13 +802,13 @@
           <t>2025-06-20</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -744,13 +816,13 @@
           <t>2025-06-21</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -758,13 +830,13 @@
           <t>2025-06-22</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -774,11 +846,19 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW AMT TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS PFE XOM MCD GE SBUX CMCSA LOW SCHW C TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+          <t>AMT</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ICE</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -788,11 +868,19 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW AMT TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS PFE XOM MCD GE CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+          <t>BX</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>SBUX</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK AMT LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -802,11 +890,19 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+          <t>ICE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>AMT</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -816,11 +912,19 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS PFE XOM MCD GE SBUX CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+          <t>SBUX</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ICE</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -828,13 +932,13 @@
           <t>2025-06-27</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS PFE XOM MCD GE SBUX CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -842,13 +946,13 @@
           <t>2025-06-28</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS PFE XOM MCD GE SBUX CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -856,13 +960,13 @@
           <t>2025-06-29</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS PFE XOM MCD GE SBUX CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
+      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -872,11 +976,19 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>PEP IBM CRWD LIN TSLA AVGO MSFT VZ BRK-B ADBE NEE CB VRTX GOOG AXP UBER META NFLX APH ADP MMC ACN T NVDA ORCL GILD ADI KLAC DE NOW TJX UNP INTU PGR WFC SYK MU LMT COP CAT QCOM HON MRK AMD WMT COF V ISRG CVX AMGN ABBV AMZN UNH BAC AAPL AMAT GOOGL COST BLK RTX PANW MDT PG PM BSX TXN BKNG JNJ LRCX DHR BA KKR KO DIS TMUS ICE PFE XOM MCD GE CMCSA LOW SCHW C BX TMO CSCO PLTR CRM ANET JPM MA ETN GS LLY ABT SPGI HD MS GEV</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+          <t>ICE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>SBUX</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Data for 1 July
</commit_message>
<xml_diff>
--- a/data/index_report.xlsx
+++ b/data/index_report.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LLY V SPGI MDT NEE C CME APH MO BAC COF INTU LOW CVX ISRG BA BLK META CRM QCOM DHR NOW KKR BRK-B COST PG GILD AVGO ABBV ORCL CMCSA MCD PEP BKNG GEV BSX AMAT SYK DIS VZ CSCO LIN GOOGL ADP LRCX ANET JNJ T AMZN PLTR DE MU LMT VRTX AMGN TXN HD PM ETN KO IBM SCHW WMT HON ADI PGR GS NVDA MSFT WFC UBER PANW JPM GOOG AAPL MMC NFLX UNH RTX ABT MA UNP MS TJX ADBE AXP XOM TMO ICE CB COP CRWD MRK PFE TSLA CAT AMD GE TMUS ACN</t>
+          <t>PM HD ADP LIN LMT KO LLY META CAT SYK AAPL PLTR CMCSA AMGN BKNG AMZN INTU TJX VRTX COF AXP ADBE GOOGL MA AMAT PFE CVX NFLX AVGO JNJ MCD UNP KKR TMUS BRK-B ADI DE MMC GE CSCO WMT VZ JPM NVDA COST GOOG BAC SPGI CRWD BLK TMO BA PGR PANW APH PG SCHW ACN MO AMD ABBV BSX UNH HON GILD ICE CB GS IBM T V NOW UBER DIS MS WFC XOM GEV ANET LRCX MRK LOW ETN MDT NEE ISRG C ORCL MU PEP MSFT CME RTX CRM TSLA DHR QCOM TXN COP ABT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -482,7 +482,7 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C CME BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH MO COF ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP CME RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN MO AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C CME BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP CME RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -620,7 +620,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -648,7 +648,7 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -692,7 +692,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -778,7 +778,7 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -792,7 +792,7 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP ICE COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD ICE GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -856,7 +856,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX SBUX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -878,7 +878,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK AMT LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMT AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV LRCX ANET LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -936,7 +936,7 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -950,7 +950,7 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -964,7 +964,7 @@
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET SBUX AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -986,7 +986,43 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>LLY V SPGI NEE C BAC INTU LOW CVX BLK QCOM DHR NOW BRK-B BX GILD AVGO ABBV ORCL PEP BKNG GEV AMAT SYK LIN JNJ T PLTR MU LMT TXN HD ETN KO IBM SCHW WMT HON GS UBER PANW JPM AAPL RTX ABT UNP XOM TMO CB MRK PFE TSLA AMD GE TMUS ACN MDT APH COF KLAC ISRG BA META CRM KKR COST PG CMCSA MCD BSX DIS VZ CSCO GOOGL ADP LRCX ANET AMZN DE VRTX AMGN PM ADI PGR NVDA MSFT WFC GOOG MMC NFLX UNH MA MS TJX ADBE AXP COP CRWD CAT</t>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SBUX</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ICE</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>PM ADP LMT LLY INTU COF AXP GOOGL MA AMAT CVX NFLX AVGO JNJ MCD UNP KLAC BRK-B ADI DE MMC SBUX VZ BAC SPGI CRWD TMO BA SCHW ABBV BSX CB IBM T V MS WFC XOM GEV ANET LRCX LOW ISRG C ORCL PEP RTX CRM TSLA DHR TXN COP HD LIN KO META CAT SYK AAPL PLTR CMCSA AMGN BKNG TJX VRTX ADBE BX PFE KKR TMUS GE CSCO WMT JPM COST GOOG NVDA BLK PGR PANW APH PG ACN AMD UNH HON GILD GS NOW UBER DIS MRK ETN MDT NEE MU MSFT QCOM AMZN ABT</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1037,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1493,6 +1529,38 @@
       </c>
       <c r="D30" t="n">
         <v>4.6324</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>105.26</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.219</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4.8615</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>105.57</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.2945</v>
+      </c>
+      <c r="D32" t="n">
+        <v>5.1704</v>
       </c>
     </row>
   </sheetData>
@@ -1506,7 +1574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1883,6 +1951,30 @@
       <c r="B31" t="inlineStr">
         <is>
           <t>NVDA,MSFT,AAPL,AMZN,META,AVGO,GOOGL,TSLA,GOOG,JPM,WMT,LLY,BRK-B,ORCL,V,NFLX,MA,XOM,COST,PG,JNJ,HD,BAC,ABBV,PLTR,KO,PM,UNH,CSCO,GE,IBM,TMUS,WFC,CRM,CVX,ABT,AMD,MS,AXP,DIS,LIN,INTU,GS,NOW,MCD,T,MRK,UBER,RTX,ISRG,TXN,BKNG,ACN,CAT,VZ,PEP,QCOM,SCHW,ADBE,BLK,SPGI,C,BSX,BA,PGR,TMO,SYK,AMGN,HON,AMAT,GEV,NEE,DHR,ETN,MU,GILD,PFE,TJX,DE,UNP,PANW,COF,CMCSA,ANET,CRWD,ADP,LRCX,LOW,APH,KKR,KLAC,ADI,CB,VRTX,COP,MDT,BX,LMT,MMC,ICE</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-07-01</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>NVDA,MSFT,AAPL,AMZN,META,AVGO,GOOGL,TSLA,GOOG,JPM,WMT,LLY,BRK-B,ORCL,V,NFLX,MA,XOM,COST,PG,JNJ,HD,BAC,ABBV,KO,UNH,PLTR,PM,TMUS,CSCO,IBM,GE,WFC,CRM,CVX,ABT,MS,AXP,LIN,DIS,AMD,INTU,GS,MCD,NOW,T,MRK,ISRG,UBER,RTX,TXN,ACN,BKNG,PEP,VZ,CAT,QCOM,ADBE,SCHW,BLK,SPGI,C,TMO,BA,AMGN,BSX,PGR,HON,SYK,NEE,AMAT,DHR,PFE,UNP,TJX,GILD,ETN,GEV,DE,COF,CMCSA,MU,PANW,LOW,ADP,ANET,LRCX,CRWD,ADI,KLAC,KKR,APH,COP,VRTX,CB,MDT,BX,LMT,SBUX,MMC</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>NVDA,MSFT,AAPL,AMZN,META,AVGO,GOOGL,TSLA,GOOG,JPM,WMT,LLY,ORCL,BRK-B,V,NFLX,MA,XOM,COST,PG,JNJ,HD,BAC,ABBV,KO,PLTR,UNH,PM,CSCO,TMUS,WFC,IBM,GE,CRM,CVX,ABT,MS,AXP,LIN,AMD,DIS,GS,INTU,MCD,NOW,MRK,T,TXN,ISRG,RTX,UBER,ACN,CAT,PEP,BKNG,VZ,QCOM,SCHW,BLK,C,TMO,SPGI,ADBE,BA,AMGN,HON,BSX,AMAT,PGR,NEE,SYK,DHR,PFE,UNP,DE,ETN,COF,TJX,GILD,GEV,MU,CMCSA,PANW,LOW,ANET,LRCX,ADP,CRWD,KLAC,ADI,KKR,COP,APH,VRTX,MDT,CB,BX,LMT,SBUX,MMC</t>
         </is>
       </c>
     </row>
@@ -1945,11 +2037,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-06-30</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>105.03</v>
+        <v>105.57</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1968,7 +2060,7 @@
         <v>-1.08</v>
       </c>
       <c r="G2" t="n">
-        <v>5.03</v>
+        <v>5.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>